<commit_message>
add the VIVA to the template
</commit_message>
<xml_diff>
--- a/data-raw/template_report.xlsx
+++ b/data-raw/template_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcuser\OneDrive\IMPROVAST\ACS\CSIemail\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C148730-14E3-40ED-9E74-DB2716F72168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58268A95-FBB3-4EA5-BF24-FCDBDF58E771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -188,6 +188,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -325,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -364,6 +371,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -737,29 +751,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="3" customWidth="1"/>
+    <col min="2" max="6" width="12.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="15" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18" style="15" customWidth="1"/>
-    <col min="11" max="12" width="11.42578125" style="3"/>
-    <col min="13" max="13" width="28.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="15" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="3"/>
+    <col min="13" max="13" width="16.5703125" style="3" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" style="3" customWidth="1"/>
     <col min="15" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="57" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -775,18 +786,18 @@
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="18" t="s">
@@ -813,6 +824,7 @@
       <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="22"/>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>

</xml_diff>